<commit_message>
FIXED duplicate message sending
</commit_message>
<xml_diff>
--- a/sms_new_mandeep.xlsx
+++ b/sms_new_mandeep.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="44">
   <si>
     <t xml:space="preserve">No.</t>
   </si>
@@ -89,6 +89,12 @@
   </si>
   <si>
     <t xml:space="preserve">13049196111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BSBT</t>
   </si>
   <si>
     <t xml:space="preserve">KAMLESH PARIKH 601 SUNFLOWER 🌻 DR PFLUGERVILLE City - Texas United States Zip code - 78660 Mob no.5127726577 Gyan Ganga International order</t>
@@ -297,7 +303,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -355,10 +361,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -450,10 +452,10 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="34.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="40.85"/>
@@ -628,39 +630,78 @@
       <c r="J7" s="5"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="6"/>
+      <c r="B8" s="7" t="n">
+        <v>45154</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="6" t="n">
+        <v>2065044242</v>
+      </c>
       <c r="H8" s="10"/>
       <c r="I8" s="4"/>
       <c r="J8" s="5"/>
       <c r="K8" s="14"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="6"/>
+      <c r="B9" s="7" t="n">
+        <v>45154</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="6" t="n">
+        <v>2065044242</v>
+      </c>
       <c r="H9" s="10"/>
       <c r="I9" s="4"/>
       <c r="J9" s="5"/>
       <c r="K9" s="14"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="B10" s="7" t="n">
+        <v>45154</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="6" t="n">
+        <v>2065044242</v>
+      </c>
       <c r="H10" s="10"/>
       <c r="I10" s="4"/>
       <c r="J10" s="5"/>
@@ -669,7 +710,7 @@
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
-      <c r="C11" s="16"/>
+      <c r="C11" s="15"/>
       <c r="D11" s="10"/>
       <c r="E11" s="8"/>
       <c r="F11" s="9"/>
@@ -703,10 +744,10 @@
       <c r="H13" s="10"/>
       <c r="I13" s="4"/>
       <c r="J13" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K13" s="14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -720,10 +761,10 @@
       <c r="H14" s="10"/>
       <c r="I14" s="4"/>
       <c r="J14" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K14" s="14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -737,10 +778,10 @@
       <c r="H15" s="10"/>
       <c r="I15" s="4"/>
       <c r="J15" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="K15" s="14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -754,10 +795,10 @@
       <c r="H16" s="10"/>
       <c r="I16" s="4"/>
       <c r="J16" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K16" s="14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -767,14 +808,14 @@
       <c r="D17" s="10"/>
       <c r="E17" s="8"/>
       <c r="F17" s="9"/>
-      <c r="G17" s="17"/>
+      <c r="G17" s="16"/>
       <c r="H17" s="10"/>
       <c r="I17" s="4"/>
       <c r="J17" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K17" s="14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -788,10 +829,10 @@
       <c r="H18" s="10"/>
       <c r="I18" s="4"/>
       <c r="J18" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="K18" s="14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -805,10 +846,10 @@
       <c r="H19" s="10"/>
       <c r="I19" s="4"/>
       <c r="J19" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K19" s="14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -822,10 +863,10 @@
       <c r="H20" s="10"/>
       <c r="I20" s="4"/>
       <c r="J20" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K20" s="14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -839,10 +880,10 @@
       <c r="H21" s="10"/>
       <c r="I21" s="4"/>
       <c r="J21" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K21" s="14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -856,10 +897,10 @@
       <c r="H22" s="10"/>
       <c r="I22" s="4"/>
       <c r="J22" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="K22" s="14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -873,10 +914,10 @@
       <c r="H23" s="10"/>
       <c r="I23" s="4"/>
       <c r="J23" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K23" s="14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -890,10 +931,10 @@
       <c r="H24" s="10"/>
       <c r="I24" s="4"/>
       <c r="J24" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K24" s="14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -907,16 +948,16 @@
       <c r="H25" s="10"/>
       <c r="I25" s="4"/>
       <c r="J25" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="K25" s="14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6"/>
       <c r="B26" s="7"/>
-      <c r="C26" s="16"/>
+      <c r="C26" s="15"/>
       <c r="D26" s="10"/>
       <c r="E26" s="8"/>
       <c r="F26" s="9"/>
@@ -924,10 +965,10 @@
       <c r="H26" s="10"/>
       <c r="I26" s="4"/>
       <c r="J26" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="K26" s="14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -941,10 +982,10 @@
       <c r="H27" s="10"/>
       <c r="I27" s="4"/>
       <c r="J27" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K27" s="14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -958,10 +999,10 @@
       <c r="H28" s="10"/>
       <c r="I28" s="4"/>
       <c r="J28" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K28" s="14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -975,10 +1016,10 @@
       <c r="H29" s="10"/>
       <c r="I29" s="4"/>
       <c r="J29" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K29" s="14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -992,10 +1033,10 @@
       <c r="H30" s="10"/>
       <c r="I30" s="4"/>
       <c r="J30" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K30" s="14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added multithread and export of file
</commit_message>
<xml_diff>
--- a/sms_new_mandeep.xlsx
+++ b/sms_new_mandeep.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="57">
   <si>
     <t xml:space="preserve">No.</t>
   </si>
@@ -88,16 +88,64 @@
     <t xml:space="preserve">13049196111</t>
   </si>
   <si>
-    <t xml:space="preserve">KAMLESH PARIKH 601 SUNFLOWER 🌻 DR PFLUGERVILLE City - Texas United States Zip code - 78660 Mob no.5127726577 Gyan Ganga International order</t>
+    <t xml:space="preserve">JKR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hina Kanjiani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2050 Cross Creek Ct Allen 75013 TX USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fnu Balan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">202 Hovis Rd Hovis Rd 28164 Nc USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amanda Father - Vazquez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">116 cypress Vallejo Ca 94590 United States</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thomas Schenck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">408 210 5th avenue south Saint Petersburg 33701 Florida United States</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mohan Passi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4631 Gresham Drive, Eldorado Hills, 95762, CA, USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mohan Passi 4631 Gresham Drive Eldorado Hills 95762 CA USA 9169330761 Way of living (English) Bangladesh</t>
   </si>
   <si>
     <t xml:space="preserve">USA</t>
   </si>
   <si>
-    <t xml:space="preserve">अपना पूरा नाम | Name Kalpana Parekh पिता का नाम | Father s Name Tansukhlal Sheth मोबाईल नंबर | Mobile Number 5135056886 गाँव का नाम | Village Name Cincinnati अपने ऐरिया (मोहल्ला) का नाम | Area Name Fairfield तहसील का नाम | Block Cincinnati जिला का नाम | District Butler county राज्य का नाम | State USA पिन कोड नंबर | Pin Code 45014 बुक का नाम | Book Name &amp; LANGUAGE ज्ञान गंगा (हिंदी)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jay jalaram Rajesh Patel 23 Cedar Meadow ln Media pa 19063 USA Phone number 6093846425 Gujarati Gyan Ganga</t>
+    <t xml:space="preserve">Anantha Bass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">202 10404 Salvia Street, Charlotte, 28277, North Carolina, USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anantha Bass 202 10404 salvia street Charlotte 28277 North Carolina United states 9804285429 Way of living (English) UNITED STATES OF AMERICA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thyagarajan Iyer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6092 Elmbridge Dr, San Jose, 95129, CA, USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thyagarajan Iyer 6092 Elmbridge Dr San Jose 95129 Ca USA 9940103805 WhatsApp Way of living (English) Bangladesh</t>
   </si>
   <si>
     <t xml:space="preserve">Chris Weston Dick Weston PO Box 185 (605 Hodges Rd), Phillipsville, CA 95559 USA Southern Humboldt County California 95559 7072232226 USA English</t>
@@ -443,10 +491,10 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="34.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="40.85"/>
@@ -625,12 +673,24 @@
       <c r="A8" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="6"/>
+      <c r="B8" s="7" t="n">
+        <v>45154</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="6" t="n">
+        <v>6509194563</v>
+      </c>
       <c r="H8" s="10"/>
       <c r="I8" s="4"/>
       <c r="J8" s="5"/>
@@ -638,12 +698,24 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="6"/>
+      <c r="B9" s="7" t="n">
+        <v>45154</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="6" t="n">
+        <v>6825577801</v>
+      </c>
       <c r="H9" s="10"/>
       <c r="I9" s="4"/>
       <c r="J9" s="5"/>
@@ -651,12 +723,24 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="6"/>
+      <c r="B10" s="7" t="n">
+        <v>45154</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="6" t="n">
+        <v>7046528713</v>
+      </c>
       <c r="H10" s="10"/>
       <c r="I10" s="4"/>
       <c r="J10" s="5"/>
@@ -664,12 +748,24 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="6"/>
+      <c r="B11" s="7" t="n">
+        <v>45154</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="6" t="n">
+        <v>70765674356</v>
+      </c>
       <c r="H11" s="10"/>
       <c r="I11" s="4"/>
       <c r="J11" s="5"/>
@@ -677,12 +773,24 @@
     </row>
     <row r="12" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="6"/>
+      <c r="B12" s="7" t="n">
+        <v>45154</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="6" t="n">
+        <v>7273310529</v>
+      </c>
       <c r="H12" s="10"/>
       <c r="I12" s="4"/>
       <c r="J12" s="5"/>
@@ -690,53 +798,89 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="6"/>
+      <c r="B13" s="7" t="n">
+        <v>45154</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="6" t="n">
+        <v>9169330761</v>
+      </c>
       <c r="H13" s="10"/>
       <c r="I13" s="4"/>
       <c r="J13" s="5" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="K13" s="14" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="6"/>
+      <c r="B14" s="7" t="n">
+        <v>45154</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="6" t="n">
+        <v>9804285429</v>
+      </c>
       <c r="H14" s="10"/>
       <c r="I14" s="4"/>
       <c r="J14" s="5" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="K14" s="14" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="6"/>
+      <c r="B15" s="7" t="n">
+        <v>45154</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="6" t="n">
+        <v>9940103805</v>
+      </c>
       <c r="H15" s="10"/>
       <c r="I15" s="4"/>
       <c r="J15" s="5" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="K15" s="14" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -750,10 +894,10 @@
       <c r="H16" s="10"/>
       <c r="I16" s="4"/>
       <c r="J16" s="5" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="K16" s="14" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -767,10 +911,10 @@
       <c r="H17" s="10"/>
       <c r="I17" s="4"/>
       <c r="J17" s="5" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="K17" s="14" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -784,10 +928,10 @@
       <c r="H18" s="10"/>
       <c r="I18" s="4"/>
       <c r="J18" s="5" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="K18" s="14" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -801,10 +945,10 @@
       <c r="H19" s="10"/>
       <c r="I19" s="4"/>
       <c r="J19" s="5" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="K19" s="14" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -818,10 +962,10 @@
       <c r="H20" s="10"/>
       <c r="I20" s="4"/>
       <c r="J20" s="5" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="K20" s="14" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -835,10 +979,10 @@
       <c r="H21" s="10"/>
       <c r="I21" s="4"/>
       <c r="J21" s="5" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="K21" s="14" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -852,10 +996,10 @@
       <c r="H22" s="10"/>
       <c r="I22" s="4"/>
       <c r="J22" s="5" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="K22" s="14" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -869,10 +1013,10 @@
       <c r="H23" s="10"/>
       <c r="I23" s="4"/>
       <c r="J23" s="5" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="K23" s="14" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -886,10 +1030,10 @@
       <c r="H24" s="10"/>
       <c r="I24" s="4"/>
       <c r="J24" s="5" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="K24" s="14" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -903,10 +1047,10 @@
       <c r="H25" s="10"/>
       <c r="I25" s="4"/>
       <c r="J25" s="5" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="K25" s="14" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -920,10 +1064,10 @@
       <c r="H26" s="10"/>
       <c r="I26" s="4"/>
       <c r="J26" s="5" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="K26" s="14" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -937,10 +1081,10 @@
       <c r="H27" s="10"/>
       <c r="I27" s="4"/>
       <c r="J27" s="5" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="K27" s="14" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -954,10 +1098,10 @@
       <c r="H28" s="10"/>
       <c r="I28" s="4"/>
       <c r="J28" s="5" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="K28" s="14" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -971,10 +1115,10 @@
       <c r="H29" s="10"/>
       <c r="I29" s="4"/>
       <c r="J29" s="5" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="K29" s="14" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -988,10 +1132,10 @@
       <c r="H30" s="10"/>
       <c r="I30" s="4"/>
       <c r="J30" s="5" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="K30" s="14" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>